<commit_message>
modified TB mort and contact rates
</commit_message>
<xml_diff>
--- a/param_files/calculated_param_gen/input_data/KZN_SA_model_parameters.xlsx
+++ b/param_files/calculated_param_gen/input_data/KZN_SA_model_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/github/epi_model_HIV_TB_KZN_SA/param_files/calculated_param_gen/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862CA0FD-7192-C345-A882-88FF60B580C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86DF13A-34E7-EA4D-885F-392140963CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1680" windowWidth="33340" windowHeight="19320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2720" yWindow="1180" windowWidth="33340" windowHeight="19320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model_matched_parameters" sheetId="1" r:id="rId1"/>
@@ -936,10 +936,10 @@
   <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="I15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1030,15 +1030,15 @@
         <v>beta_1</v>
       </c>
       <c r="I2" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J2" s="5">
         <f>I2*0.75</f>
-        <v>8.25</v>
+        <v>9</v>
       </c>
       <c r="K2" s="5">
         <f>I2*1.25</f>
-        <v>13.75</v>
+        <v>15</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>87</v>
@@ -1070,15 +1070,15 @@
         <v>beta_2</v>
       </c>
       <c r="I3" s="24">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J3" s="5">
         <f>I3*0.75</f>
-        <v>8.25</v>
+        <v>9</v>
       </c>
       <c r="K3" s="5">
         <f>I3*1.25</f>
-        <v>13.75</v>
+        <v>15</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>87</v>
@@ -2354,7 +2354,7 @@
       <c r="N36" s="15"/>
       <c r="O36" s="16"/>
     </row>
-    <row r="37" spans="1:15" ht="34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:15" ht="17" x14ac:dyDescent="0.15">
       <c r="A37" s="26" t="s">
         <v>106</v>
       </c>
@@ -2409,15 +2409,15 @@
         <v>risk.other_3,</v>
       </c>
       <c r="I38" s="25">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J38" s="5">
         <f>I38*0.75</f>
-        <v>22.5</v>
+        <v>21</v>
       </c>
       <c r="K38" s="5">
         <f>I38*1.25</f>
-        <v>37.5</v>
+        <v>35</v>
       </c>
       <c r="L38" s="6" t="s">
         <v>87</v>
@@ -2444,15 +2444,15 @@
         <v>risk.other_4,</v>
       </c>
       <c r="I39" s="25">
-        <v>1.35</v>
+        <v>1.34</v>
       </c>
       <c r="J39" s="5">
         <f>I39*0.75</f>
-        <v>1.0125000000000002</v>
+        <v>1.0050000000000001</v>
       </c>
       <c r="K39" s="5">
         <f>I39*1.25</f>
-        <v>1.6875</v>
+        <v>1.675</v>
       </c>
       <c r="L39" s="6" t="s">
         <v>87</v>
@@ -2608,15 +2608,15 @@
         <v>risk.TB_2,</v>
       </c>
       <c r="I44" s="24">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J44" s="5">
         <f>I44*0.75</f>
-        <v>20.25</v>
+        <v>19.5</v>
       </c>
       <c r="K44" s="5">
         <f>I44*1.25</f>
-        <v>33.75</v>
+        <v>32.5</v>
       </c>
       <c r="L44" s="6" t="s">
         <v>87</v>
@@ -2643,15 +2643,15 @@
         <v>risk.TB_3,</v>
       </c>
       <c r="I45" s="24">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J45" s="5">
         <f>I45*0.75</f>
-        <v>38.25</v>
+        <v>39</v>
       </c>
       <c r="K45" s="5">
         <f>I45*1.25</f>
-        <v>63.75</v>
+        <v>65</v>
       </c>
       <c r="L45" s="6" t="s">
         <v>87</v>

</xml_diff>

<commit_message>
before reorg with hyak code
</commit_message>
<xml_diff>
--- a/param_files/calculated_param_gen/input_data/KZN_SA_model_parameters.xlsx
+++ b/param_files/calculated_param_gen/input_data/KZN_SA_model_parameters.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/github/epi_model_HIV_TB_KZN_SA/param_files/calculated_param_gen/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86DF13A-34E7-EA4D-885F-392140963CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7D2C37-79BF-D940-8EEF-6CECE9879C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2720" yWindow="1180" windowWidth="33340" windowHeight="19320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1100" yWindow="1340" windowWidth="33340" windowHeight="19320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model_matched_parameters" sheetId="1" r:id="rId1"/>
     <sheet name="set_ref" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">model_matched_parameters!$A$1:$O$46</definedName>
-    <definedName name="Epidemiological_data_point__description">model_matched_parameters!$A$1:$O$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">model_matched_parameters!$A$1:$O$45</definedName>
+    <definedName name="Epidemiological_data_point__description">model_matched_parameters!$A$1:$O$41</definedName>
     <definedName name="G_SET">set_ref!$A$21:$B$23</definedName>
     <definedName name="HIV_SET">set_ref!$A$15:$B$19</definedName>
     <definedName name="indirect_model_parameters">#REF!</definedName>
     <definedName name="indirect_model_params">#REF!</definedName>
-    <definedName name="model_matched_parameters">model_matched_parameters!$H$1:$I$42</definedName>
+    <definedName name="model_matched_parameters">model_matched_parameters!$H$1:$I$41</definedName>
     <definedName name="P_SET">set_ref!$A$25:$B$34</definedName>
     <definedName name="R_SET">set_ref!$A$11:$B$13</definedName>
     <definedName name="TB_SET">set_ref!$A$1:$B$9</definedName>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="120">
   <si>
     <t>Epidemiological data point (description)</t>
   </si>
@@ -379,9 +379,6 @@
     <t>Rate of exits from the population due to aging</t>
   </si>
   <si>
-    <t>Fraction of new TB infections that are MDR-TB for males</t>
-  </si>
-  <si>
     <t>mu.baselinefactor</t>
   </si>
   <si>
@@ -407,6 +404,9 @@
   </si>
   <si>
     <t>G_compartment</t>
+  </si>
+  <si>
+    <t>Fraction of new TB infections that are MDR-TB</t>
   </si>
 </sst>
 </file>
@@ -933,13 +933,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="8" ySplit="1" topLeftCell="I26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -975,16 +975,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>81</v>
@@ -1026,19 +1026,19 @@
         <v>1</v>
       </c>
       <c r="H2" s="5" t="str">
-        <f t="shared" ref="H2:H46" si="0">CONCATENATE(B2,"_",D2,IF(D2&lt;&gt;"",",",""),E2,IF(E2&lt;&gt;"",",",""),F2,IF(F2&lt;&gt;"",",",""),G2)</f>
+        <f t="shared" ref="H2:H45" si="0">CONCATENATE(B2,"_",D2,IF(D2&lt;&gt;"",",",""),E2,IF(E2&lt;&gt;"",",",""),F2,IF(F2&lt;&gt;"",",",""),G2)</f>
         <v>beta_1</v>
       </c>
       <c r="I2" s="24">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J2" s="5">
         <f>I2*0.75</f>
-        <v>9</v>
+        <v>10.5</v>
       </c>
       <c r="K2" s="5">
         <f>I2*1.25</f>
-        <v>15</v>
+        <v>17.5</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>87</v>
@@ -1070,15 +1070,15 @@
         <v>beta_2</v>
       </c>
       <c r="I3" s="24">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J3" s="5">
         <f>I3*0.75</f>
-        <v>9</v>
+        <v>10.5</v>
       </c>
       <c r="K3" s="5">
         <f>I3*1.25</f>
-        <v>15</v>
+        <v>17.5</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>87</v>
@@ -1145,11 +1145,11 @@
         <v>0.9</v>
       </c>
       <c r="J5" s="5">
-        <f t="shared" ref="J5:J10" si="1">I5*0.75</f>
+        <f t="shared" ref="J5:J9" si="1">I5*0.75</f>
         <v>0.67500000000000004</v>
       </c>
       <c r="K5" s="5">
-        <f t="shared" ref="K5:K10" si="2">I5*1.25</f>
+        <f t="shared" ref="K5:K9" si="2">I5*1.25</f>
         <v>1.125</v>
       </c>
       <c r="L5" s="6" t="s">
@@ -1249,7 +1249,7 @@
     </row>
     <row r="8" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
@@ -1258,12 +1258,9 @@
         <v>7</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="G8" s="5">
-        <v>1</v>
-      </c>
       <c r="H8" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>varepsilon_1</v>
+        <v>varepsilon_</v>
       </c>
       <c r="I8" s="24">
         <v>3.6999999999999998E-2</v>
@@ -1290,44 +1287,50 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
-        <v>110</v>
+      <c r="A9" s="26" t="s">
+        <v>92</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C9" s="30">
         <v>8</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="G9" s="5">
-        <v>2</v>
+      <c r="E9" s="5">
+        <v>1</v>
       </c>
       <c r="H9" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>varepsilon_2</v>
-      </c>
-      <c r="I9" s="24">
-        <v>3.6999999999999998E-2</v>
+        <v>iota_1,</v>
+      </c>
+      <c r="I9" s="27">
+        <v>0.43</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="1"/>
-        <v>2.7749999999999997E-2</v>
+        <v>0.32250000000000001</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" si="2"/>
-        <v>4.6249999999999999E-2</v>
+        <v>0.53749999999999998</v>
       </c>
       <c r="L9" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="M9" s="14"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="16"/>
+      <c r="M9" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="N9" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="10" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>9</v>
@@ -1337,76 +1340,73 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="5">
+        <v>2</v>
+      </c>
+      <c r="H10" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>iota_2,</v>
+      </c>
+      <c r="I10" s="27">
         <v>1</v>
       </c>
-      <c r="H10" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>iota_1,</v>
-      </c>
-      <c r="I10" s="27">
-        <v>0.67</v>
-      </c>
-      <c r="J10" s="5">
-        <f t="shared" si="1"/>
-        <v>0.50250000000000006</v>
-      </c>
-      <c r="K10" s="5">
-        <f t="shared" si="2"/>
-        <v>0.83750000000000002</v>
-      </c>
       <c r="L10" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O10" s="16" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
-        <v>93</v>
+      <c r="A11" s="23" t="s">
+        <v>79</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="C11" s="30">
         <v>10</v>
       </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="5">
-        <v>2</v>
-      </c>
       <c r="H11" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>iota_2,</v>
+        <v>xi_</v>
       </c>
       <c r="I11" s="27">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="J11" s="5">
+        <f>I11*0.75</f>
+        <v>3</v>
+      </c>
+      <c r="K11" s="5">
+        <f>I11*1.25</f>
+        <v>5</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="N11" s="15" t="s">
-        <v>66</v>
+        <v>70</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>67</v>
       </c>
       <c r="O11" s="16" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
-        <v>79</v>
+      <c r="A12" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="C12" s="30">
         <v>11</v>
@@ -1414,38 +1414,34 @@
       <c r="D12" s="4"/>
       <c r="H12" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>xi_</v>
+        <v>zeta_</v>
       </c>
       <c r="I12" s="27">
-        <v>4</v>
+        <v>0.4</v>
       </c>
       <c r="J12" s="5">
         <f>I12*0.75</f>
-        <v>3</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="K12" s="5">
-        <f>I12*1.25</f>
-        <v>5</v>
+        <f>I12*(1.25)</f>
+        <v>0.5</v>
       </c>
       <c r="L12" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="M12" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="N12" s="19" t="s">
-        <v>67</v>
-      </c>
+      <c r="M12" s="14"/>
+      <c r="N12" s="15"/>
       <c r="O12" s="16" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
-        <v>16</v>
+      <c r="A13" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C13" s="30">
         <v>12</v>
@@ -1453,21 +1449,13 @@
       <c r="D13" s="4"/>
       <c r="H13" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>zeta_</v>
-      </c>
-      <c r="I13" s="27">
-        <v>0.4</v>
-      </c>
-      <c r="J13" s="5">
-        <f>I13*0.75</f>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="K13" s="5">
-        <f>I13*(1.25)</f>
-        <v>0.5</v>
+        <v>omega_</v>
+      </c>
+      <c r="I13" s="24">
+        <v>2</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M13" s="14"/>
       <c r="N13" s="15"/>
@@ -1476,35 +1464,42 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
-        <v>54</v>
+      <c r="A14" s="26" t="s">
+        <v>96</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" s="30">
         <v>13</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="4">
+        <v>34</v>
+      </c>
       <c r="H14" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>omega_</v>
-      </c>
-      <c r="I14" s="24">
-        <v>2</v>
+        <v>pi_34,</v>
+      </c>
+      <c r="I14" s="25">
+        <f>1/2</f>
+        <v>0.5</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="M14" s="14"/>
-      <c r="N14" s="15"/>
+      <c r="M14" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="N14" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="O14" s="16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="26" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>22</v>
@@ -1513,17 +1508,25 @@
         <v>14</v>
       </c>
       <c r="D15" s="4">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H15" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>pi_34,</v>
+        <v>pi_36,</v>
       </c>
       <c r="I15" s="25">
-        <v>0.5</v>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" ref="J15:J21" si="3">I15*0.75</f>
+        <v>1.8750000000000003E-2</v>
+      </c>
+      <c r="K15" s="5">
+        <f t="shared" ref="K15:K21" si="4">I15*1.25</f>
+        <v>3.125E-2</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M15" s="5" t="s">
         <v>80</v>
@@ -1537,7 +1540,7 @@
     </row>
     <row r="16" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>22</v>
@@ -1546,22 +1549,22 @@
         <v>15</v>
       </c>
       <c r="D16" s="4">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H16" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>pi_36,</v>
+        <v>pi_46,</v>
       </c>
       <c r="I16" s="25">
-        <v>2.5000000000000001E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="J16" s="5">
-        <f t="shared" ref="J16:J22" si="3">I16*0.75</f>
-        <v>1.8750000000000003E-2</v>
+        <f t="shared" si="3"/>
+        <v>7.5000000000000002E-4</v>
       </c>
       <c r="K16" s="5">
-        <f t="shared" ref="K16:K22" si="4">I16*1.25</f>
-        <v>3.125E-2</v>
+        <f t="shared" si="4"/>
+        <v>1.25E-3</v>
       </c>
       <c r="L16" s="6" t="s">
         <v>87</v>
@@ -1570,48 +1573,41 @@
         <v>80</v>
       </c>
       <c r="N16" s="15" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="O16" s="16" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="48" x14ac:dyDescent="0.2">
-      <c r="A17" s="26" t="s">
-        <v>98</v>
+      <c r="A17" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C17" s="30">
         <v>16</v>
       </c>
-      <c r="D17" s="4">
-        <v>46</v>
+      <c r="D17" s="4"/>
+      <c r="F17" s="5">
+        <v>1</v>
       </c>
       <c r="H17" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>pi_46,</v>
-      </c>
-      <c r="I17" s="25">
-        <v>1E-3</v>
-      </c>
-      <c r="J17" s="5">
-        <f t="shared" si="3"/>
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K17" s="5">
-        <f t="shared" si="4"/>
-        <v>1.25E-3</v>
+        <v>theta_1,</v>
+      </c>
+      <c r="I17" s="24">
+        <v>1</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M17" s="5" t="s">
         <v>80</v>
       </c>
       <c r="N17" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O17" s="16" t="s">
         <v>87</v>
@@ -1619,7 +1615,7 @@
     </row>
     <row r="18" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>25</v>
@@ -1629,31 +1625,37 @@
       </c>
       <c r="D18" s="4"/>
       <c r="F18" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H18" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>theta_1,</v>
+        <v>theta_2,</v>
       </c>
       <c r="I18" s="24">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="J18" s="5">
+        <f t="shared" si="3"/>
+        <v>7.5</v>
+      </c>
+      <c r="K18" s="5">
+        <f t="shared" si="4"/>
+        <v>12.5</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M18" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="N18" s="15" t="s">
-        <v>72</v>
-      </c>
+      <c r="N18" s="15"/>
       <c r="O18" s="16" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>25</v>
@@ -1663,22 +1665,22 @@
       </c>
       <c r="D19" s="4"/>
       <c r="F19" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H19" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>theta_2,</v>
+        <v>theta_3,</v>
       </c>
       <c r="I19" s="24">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="J19" s="5">
         <f t="shared" si="3"/>
-        <v>7.5</v>
+        <v>12.75</v>
       </c>
       <c r="K19" s="5">
         <f t="shared" si="4"/>
-        <v>12.5</v>
+        <v>21.25</v>
       </c>
       <c r="L19" s="6" t="s">
         <v>87</v>
@@ -1693,7 +1695,7 @@
     </row>
     <row r="20" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>25</v>
@@ -1703,22 +1705,22 @@
       </c>
       <c r="D20" s="4"/>
       <c r="F20" s="5">
+        <v>4</v>
+      </c>
+      <c r="H20" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>theta_4,</v>
+      </c>
+      <c r="I20" s="24">
         <v>3</v>
-      </c>
-      <c r="H20" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>theta_3,</v>
-      </c>
-      <c r="I20" s="24">
-        <v>17</v>
       </c>
       <c r="J20" s="5">
         <f t="shared" si="3"/>
-        <v>12.75</v>
+        <v>2.25</v>
       </c>
       <c r="K20" s="5">
         <f t="shared" si="4"/>
-        <v>21.25</v>
+        <v>3.75</v>
       </c>
       <c r="L20" s="6" t="s">
         <v>87</v>
@@ -1733,32 +1735,31 @@
     </row>
     <row r="21" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C21" s="30">
         <v>20</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="F21" s="5">
-        <v>4</v>
+      <c r="D21" s="4">
+        <v>56</v>
       </c>
       <c r="H21" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>theta_4,</v>
-      </c>
-      <c r="I21" s="24">
-        <v>3</v>
+        <v>pi_56,</v>
+      </c>
+      <c r="I21" s="25">
+        <v>3.3E-3</v>
       </c>
       <c r="J21" s="5">
         <f t="shared" si="3"/>
-        <v>2.25</v>
+        <v>2.4749999999999998E-3</v>
       </c>
       <c r="K21" s="5">
         <f t="shared" si="4"/>
-        <v>3.75</v>
+        <v>4.1250000000000002E-3</v>
       </c>
       <c r="L21" s="6" t="s">
         <v>87</v>
@@ -1772,47 +1773,43 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="48" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="4" t="s">
+      <c r="A22" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="30">
         <v>21</v>
       </c>
-      <c r="D22" s="4">
-        <v>56</v>
+      <c r="D22" s="5">
+        <v>67</v>
       </c>
       <c r="H22" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>pi_56,</v>
+        <v>pi_67,</v>
       </c>
       <c r="I22" s="25">
-        <v>3.3E-3</v>
-      </c>
-      <c r="J22" s="5">
-        <f t="shared" si="3"/>
-        <v>2.4749999999999998E-3</v>
-      </c>
-      <c r="K22" s="5">
-        <f t="shared" si="4"/>
-        <v>4.1250000000000002E-3</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
       <c r="L22" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M22" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="N22" s="15"/>
+      <c r="N22" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="O22" s="16" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="48" x14ac:dyDescent="0.2">
-      <c r="A23" s="26" t="s">
-        <v>100</v>
+    <row r="23" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="21" t="s">
+        <v>71</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>22</v>
@@ -1821,19 +1818,25 @@
         <v>22</v>
       </c>
       <c r="D23" s="5">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="H23" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>pi_67,</v>
+        <v>pi_86,</v>
       </c>
       <c r="I23" s="25">
-        <v>2</v>
-      </c>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
+        <v>3.3E-3</v>
+      </c>
+      <c r="J23" s="5">
+        <f t="shared" ref="J23:J34" si="5">I23*0.75</f>
+        <v>2.4749999999999998E-3</v>
+      </c>
+      <c r="K23" s="5">
+        <f t="shared" ref="K23:K34" si="6">I23*1.25</f>
+        <v>4.1250000000000002E-3</v>
+      </c>
       <c r="L23" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M23" s="5" t="s">
         <v>80</v>
@@ -1846,32 +1849,34 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>22</v>
+      <c r="A24" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C24" s="30">
         <v>23</v>
       </c>
-      <c r="D24" s="5">
-        <v>86</v>
+      <c r="D24" s="4"/>
+      <c r="F24" s="5">
+        <v>1</v>
       </c>
       <c r="H24" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>pi_86,</v>
-      </c>
-      <c r="I24" s="25">
-        <v>3.3E-3</v>
+        <v>upsilon_1,</v>
+      </c>
+      <c r="I24" s="24">
+        <f>0.25</f>
+        <v>0.25</v>
       </c>
       <c r="J24" s="5">
-        <f t="shared" ref="J24:J35" si="5">I24*0.75</f>
-        <v>2.4749999999999998E-3</v>
+        <f t="shared" si="5"/>
+        <v>0.1875</v>
       </c>
       <c r="K24" s="5">
-        <f t="shared" ref="K24:K35" si="6">I24*1.25</f>
-        <v>4.1250000000000002E-3</v>
+        <f t="shared" si="6"/>
+        <v>0.3125</v>
       </c>
       <c r="L24" s="6" t="s">
         <v>87</v>
@@ -1880,7 +1885,7 @@
         <v>80</v>
       </c>
       <c r="N24" s="15" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="O24" s="16" t="s">
         <v>87</v>
@@ -1888,7 +1893,7 @@
     </row>
     <row r="25" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>15</v>
@@ -1898,23 +1903,23 @@
       </c>
       <c r="D25" s="4"/>
       <c r="F25" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H25" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>upsilon_1,</v>
+        <v>upsilon_2,</v>
       </c>
       <c r="I25" s="24">
-        <f>0.25</f>
-        <v>0.25</v>
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J25" s="5">
         <f t="shared" si="5"/>
-        <v>0.1875</v>
+        <v>0.25</v>
       </c>
       <c r="K25" s="5">
         <f t="shared" si="6"/>
-        <v>0.3125</v>
+        <v>0.41666666666666663</v>
       </c>
       <c r="L25" s="6" t="s">
         <v>87</v>
@@ -1929,9 +1934,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>15</v>
@@ -1941,14 +1946,14 @@
       </c>
       <c r="D26" s="4"/>
       <c r="F26" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H26" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>upsilon_2,</v>
+        <v>upsilon_3,</v>
       </c>
       <c r="I26" s="24">
-        <f>1/3</f>
+        <f t="shared" ref="I26:I27" si="7">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="J26" s="5">
@@ -1965,16 +1970,14 @@
       <c r="M26" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="N26" s="15" t="s">
-        <v>72</v>
-      </c>
+      <c r="N26" s="15"/>
       <c r="O26" s="16" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>15</v>
@@ -1984,14 +1987,14 @@
       </c>
       <c r="D27" s="4"/>
       <c r="F27" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H27" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>upsilon_3,</v>
+        <v>upsilon_4,</v>
       </c>
       <c r="I27" s="24">
-        <f>1/3</f>
+        <f t="shared" si="7"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J27" s="5">
@@ -2014,34 +2017,32 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="48" x14ac:dyDescent="0.2">
-      <c r="A28" s="22" t="s">
-        <v>78</v>
+      <c r="A28" s="20" t="s">
+        <v>69</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C28" s="30">
         <v>27</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="F28" s="5">
-        <v>4</v>
+      <c r="D28" s="4">
+        <v>76</v>
       </c>
       <c r="H28" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>upsilon_4,</v>
-      </c>
-      <c r="I28" s="24">
-        <f>1/3</f>
-        <v>0.33333333333333331</v>
+        <v>pi_76,</v>
+      </c>
+      <c r="I28" s="25">
+        <v>0.01</v>
       </c>
       <c r="J28" s="5">
         <f t="shared" si="5"/>
-        <v>0.25</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="K28" s="5">
         <f t="shared" si="6"/>
-        <v>0.41666666666666663</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="L28" s="6" t="s">
         <v>87</v>
@@ -2054,62 +2055,58 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="48" x14ac:dyDescent="0.2">
-      <c r="A29" s="20" t="s">
-        <v>69</v>
+    <row r="29" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="26" t="s">
+        <v>101</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
       <c r="C29" s="30">
         <v>28</v>
       </c>
-      <c r="D29" s="4">
-        <v>76</v>
+      <c r="D29" s="4"/>
+      <c r="G29" s="5">
+        <v>1</v>
       </c>
       <c r="H29" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>pi_76,</v>
+        <v>eta.baselinefactor_1</v>
       </c>
       <c r="I29" s="25">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="J29" s="5">
         <f t="shared" si="5"/>
-        <v>7.4999999999999997E-3</v>
+        <v>0.75</v>
       </c>
       <c r="K29" s="5">
         <f t="shared" si="6"/>
-        <v>1.2500000000000001E-2</v>
+        <v>1.25</v>
       </c>
       <c r="L29" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="M29" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="N29" s="15"/>
-      <c r="O29" s="16" t="s">
-        <v>87</v>
-      </c>
+      <c r="O29" s="16"/>
     </row>
     <row r="30" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="26" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C30" s="30">
         <v>29</v>
       </c>
       <c r="D30" s="4"/>
       <c r="G30" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>eta.baselinefactor_1</v>
+        <v>eta.baselinefactor_2</v>
       </c>
       <c r="I30" s="25">
         <v>1</v>
@@ -2128,44 +2125,55 @@
       <c r="N30" s="15"/>
       <c r="O30" s="16"/>
     </row>
-    <row r="31" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="26" t="s">
-        <v>102</v>
+    <row r="31" spans="1:15" ht="51" x14ac:dyDescent="0.15">
+      <c r="A31" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>115</v>
+        <v>29</v>
       </c>
       <c r="C31" s="30">
         <v>30</v>
       </c>
       <c r="D31" s="4"/>
+      <c r="F31" s="5">
+        <v>23</v>
+      </c>
       <c r="G31" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H31" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>eta.baselinefactor_2</v>
-      </c>
-      <c r="I31" s="25">
-        <v>1</v>
+        <v>eta_23,1</v>
+      </c>
+      <c r="I31" s="27">
+        <f>1/(0.25+1.71+1.05+4.71)</f>
+        <v>0.1295336787564767</v>
       </c>
       <c r="J31" s="5">
         <f t="shared" si="5"/>
-        <v>0.75</v>
+        <v>9.7150259067357525E-2</v>
       </c>
       <c r="K31" s="5">
         <f t="shared" si="6"/>
-        <v>1.25</v>
+        <v>0.16191709844559588</v>
       </c>
       <c r="L31" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="N31" s="15"/>
-      <c r="O31" s="16"/>
+      <c r="M31" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="N31" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="O31" s="16" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="32" spans="1:15" ht="51" x14ac:dyDescent="0.15">
       <c r="A32" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>29</v>
@@ -2178,23 +2186,22 @@
         <v>23</v>
       </c>
       <c r="G32" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H32" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>eta_23,1</v>
+        <v>eta_23,2</v>
       </c>
       <c r="I32" s="27">
-        <f>1/(0.25+1.71+1.05+4.71)</f>
-        <v>0.1295336787564767</v>
+        <v>9.7560975609756101E-2</v>
       </c>
       <c r="J32" s="5">
         <f t="shared" si="5"/>
-        <v>9.7150259067357525E-2</v>
+        <v>7.3170731707317083E-2</v>
       </c>
       <c r="K32" s="5">
         <f t="shared" si="6"/>
-        <v>0.16191709844559588</v>
+        <v>0.12195121951219512</v>
       </c>
       <c r="L32" s="6" t="s">
         <v>87</v>
@@ -2203,74 +2210,65 @@
         <v>59</v>
       </c>
       <c r="N32" s="15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O32" s="16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="51" x14ac:dyDescent="0.15">
-      <c r="A33" s="12" t="s">
-        <v>56</v>
+    <row r="33" spans="1:15" ht="17" x14ac:dyDescent="0.15">
+      <c r="A33" s="26" t="s">
+        <v>103</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>29</v>
+        <v>110</v>
       </c>
       <c r="C33" s="30">
         <v>32</v>
       </c>
       <c r="D33" s="4"/>
-      <c r="F33" s="5">
-        <v>23</v>
-      </c>
       <c r="G33" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H33" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>eta_23,2</v>
+        <v>mu.baselinefactor_1</v>
       </c>
       <c r="I33" s="27">
-        <v>9.7560975609756101E-2</v>
+        <v>1</v>
       </c>
       <c r="J33" s="5">
         <f t="shared" si="5"/>
-        <v>7.3170731707317083E-2</v>
+        <v>0.75</v>
       </c>
       <c r="K33" s="5">
         <f t="shared" si="6"/>
-        <v>0.12195121951219512</v>
+        <v>1.25</v>
       </c>
       <c r="L33" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="M33" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="N33" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="O33" s="16" t="s">
-        <v>86</v>
-      </c>
+      <c r="M33" s="17"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="16"/>
     </row>
     <row r="34" spans="1:15" ht="17" x14ac:dyDescent="0.15">
       <c r="A34" s="26" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C34" s="30">
         <v>33</v>
       </c>
       <c r="D34" s="4"/>
       <c r="G34" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H34" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>mu.baselinefactor_1</v>
+        <v>mu.baselinefactor_2</v>
       </c>
       <c r="I34" s="27">
         <v>1</v>
@@ -2292,7 +2290,7 @@
     </row>
     <row r="35" spans="1:15" ht="17" x14ac:dyDescent="0.15">
       <c r="A35" s="26" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>111</v>
@@ -2301,123 +2299,122 @@
         <v>34</v>
       </c>
       <c r="D35" s="4"/>
-      <c r="G35" s="5">
-        <v>2</v>
+      <c r="F35" s="5">
+        <v>1</v>
       </c>
       <c r="H35" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>mu.baselinefactor_2</v>
+        <v>risk.other_1,</v>
       </c>
       <c r="I35" s="27">
         <v>1</v>
       </c>
-      <c r="J35" s="5">
-        <f t="shared" si="5"/>
-        <v>0.75</v>
-      </c>
-      <c r="K35" s="5">
-        <f t="shared" si="6"/>
-        <v>1.25</v>
-      </c>
       <c r="L35" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M35" s="17"/>
       <c r="N35" s="15"/>
       <c r="O35" s="16"/>
     </row>
-    <row r="36" spans="1:15" ht="17" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:15" ht="34" x14ac:dyDescent="0.15">
       <c r="A36" s="26" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C36" s="30">
         <v>35</v>
       </c>
       <c r="D36" s="4"/>
       <c r="F36" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H36" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>risk.other_1,</v>
+        <v>risk.other_2,</v>
       </c>
       <c r="I36" s="27">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="J36" s="5">
+        <f>I36*0.75</f>
+        <v>6</v>
+      </c>
+      <c r="K36" s="5">
+        <f>I36*1.25</f>
+        <v>10</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M36" s="17"/>
       <c r="N36" s="15"/>
       <c r="O36" s="16"/>
     </row>
-    <row r="37" spans="1:15" ht="17" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="26" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C37" s="30">
         <v>36</v>
       </c>
       <c r="D37" s="4"/>
       <c r="F37" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H37" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>risk.other_2,</v>
-      </c>
-      <c r="I37" s="27">
-        <v>8</v>
+        <v>risk.other_3,</v>
+      </c>
+      <c r="I37" s="25">
+        <v>26</v>
       </c>
       <c r="J37" s="5">
         <f>I37*0.75</f>
-        <v>6</v>
+        <v>19.5</v>
       </c>
       <c r="K37" s="5">
         <f>I37*1.25</f>
-        <v>10</v>
+        <v>32.5</v>
       </c>
       <c r="L37" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="M37" s="17"/>
       <c r="N37" s="15"/>
       <c r="O37" s="16"/>
     </row>
-    <row r="38" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="26" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C38" s="30">
         <v>37</v>
       </c>
       <c r="D38" s="4"/>
       <c r="F38" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H38" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>risk.other_3,</v>
+        <v>risk.other_4,</v>
       </c>
       <c r="I38" s="25">
-        <v>28</v>
+        <v>1.35</v>
       </c>
       <c r="J38" s="5">
         <f>I38*0.75</f>
-        <v>21</v>
+        <v>1.0125000000000002</v>
       </c>
       <c r="K38" s="5">
         <f>I38*1.25</f>
-        <v>35</v>
+        <v>1.6875</v>
       </c>
       <c r="L38" s="6" t="s">
         <v>87</v>
@@ -2425,40 +2422,37 @@
       <c r="N38" s="15"/>
       <c r="O38" s="16"/>
     </row>
-    <row r="39" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="26" t="s">
-        <v>108</v>
+    <row r="39" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="A39" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>112</v>
+        <v>20</v>
       </c>
       <c r="C39" s="30">
         <v>38</v>
       </c>
       <c r="D39" s="4"/>
-      <c r="F39" s="5">
-        <v>4</v>
+      <c r="E39" s="5">
+        <v>1</v>
       </c>
       <c r="H39" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>risk.other_4,</v>
-      </c>
-      <c r="I39" s="25">
-        <v>1.34</v>
-      </c>
-      <c r="J39" s="5">
-        <f>I39*0.75</f>
-        <v>1.0050000000000001</v>
-      </c>
-      <c r="K39" s="5">
-        <f>I39*1.25</f>
-        <v>1.675</v>
+        <v>gamma_1,</v>
+      </c>
+      <c r="I39" s="24">
+        <v>1</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="N39" s="15"/>
-      <c r="O39" s="16"/>
+      <c r="O39" s="16" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="40" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
@@ -2472,14 +2466,14 @@
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H40" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>gamma_1,</v>
+        <v>gamma_2,</v>
       </c>
       <c r="I40" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L40" s="6" t="s">
         <v>86</v>
@@ -2487,48 +2481,45 @@
       <c r="M40" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="N40" s="15"/>
+      <c r="N40" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="O40" s="16" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="48" x14ac:dyDescent="0.2">
-      <c r="A41" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>20</v>
+      <c r="A41" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="C41" s="30">
         <v>40</v>
       </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="5">
-        <v>2</v>
-      </c>
       <c r="H41" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>gamma_2,</v>
-      </c>
-      <c r="I41" s="24">
-        <v>0</v>
+        <v>alpha.out_</v>
+      </c>
+      <c r="I41" s="27">
+        <f>1/(60-15)</f>
+        <v>2.2222222222222223E-2</v>
       </c>
       <c r="L41" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="M41" s="5" t="s">
-        <v>80</v>
-      </c>
+      <c r="M41" s="14"/>
       <c r="N41" s="15" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="O41" s="16" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>113</v>
@@ -2536,52 +2527,58 @@
       <c r="C42" s="30">
         <v>41</v>
       </c>
+      <c r="F42" s="5">
+        <v>1</v>
+      </c>
       <c r="H42" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>alpha.out_</v>
-      </c>
-      <c r="I42" s="27">
-        <f>1/(60-15)</f>
-        <v>2.2222222222222223E-2</v>
+        <v>risk.TB_1,</v>
+      </c>
+      <c r="I42" s="24">
+        <v>15.5</v>
+      </c>
+      <c r="J42" s="5">
+        <f>I42*0.75</f>
+        <v>11.625</v>
+      </c>
+      <c r="K42" s="5">
+        <f>I42*1.25</f>
+        <v>19.375</v>
       </c>
       <c r="L42" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="O42" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="M42" s="14"/>
-      <c r="N42" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="O42" s="16" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C43" s="30">
         <v>42</v>
       </c>
       <c r="F43" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H43" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>risk.TB_1,</v>
+        <v>risk.TB_2,</v>
       </c>
       <c r="I43" s="24">
-        <v>16.5</v>
+        <v>26</v>
       </c>
       <c r="J43" s="5">
         <f>I43*0.75</f>
-        <v>12.375</v>
+        <v>19.5</v>
       </c>
       <c r="K43" s="5">
         <f>I43*1.25</f>
-        <v>20.625</v>
+        <v>32.5</v>
       </c>
       <c r="L43" s="6" t="s">
         <v>87</v>
@@ -2592,31 +2589,31 @@
     </row>
     <row r="44" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C44" s="30">
         <v>43</v>
       </c>
       <c r="F44" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H44" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>risk.TB_2,</v>
+        <v>risk.TB_3,</v>
       </c>
       <c r="I44" s="24">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="J44" s="5">
         <f>I44*0.75</f>
-        <v>19.5</v>
+        <v>37.5</v>
       </c>
       <c r="K44" s="5">
         <f>I44*1.25</f>
-        <v>32.5</v>
+        <v>62.5</v>
       </c>
       <c r="L44" s="6" t="s">
         <v>87</v>
@@ -2627,31 +2624,31 @@
     </row>
     <row r="45" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C45" s="30">
         <v>44</v>
       </c>
       <c r="F45" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H45" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>risk.TB_3,</v>
+        <v>risk.TB_4,</v>
       </c>
       <c r="I45" s="24">
-        <v>52</v>
+        <v>18.5</v>
       </c>
       <c r="J45" s="5">
         <f>I45*0.75</f>
-        <v>39</v>
+        <v>13.875</v>
       </c>
       <c r="K45" s="5">
         <f>I45*1.25</f>
-        <v>65</v>
+        <v>23.125</v>
       </c>
       <c r="L45" s="6" t="s">
         <v>87</v>
@@ -2660,44 +2657,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C46" s="30">
-        <v>45</v>
-      </c>
-      <c r="F46" s="5">
-        <v>4</v>
-      </c>
-      <c r="H46" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>risk.TB_4,</v>
-      </c>
-      <c r="I46" s="24">
-        <v>19.5</v>
-      </c>
-      <c r="J46" s="5">
-        <f>I46*0.75</f>
-        <v>14.625</v>
-      </c>
-      <c r="K46" s="5">
-        <f>I46*1.25</f>
-        <v>24.375</v>
-      </c>
-      <c r="L46" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="O46" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K46">
-    <sortCondition ref="C2:C46"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K45">
+    <sortCondition ref="C2:C45"/>
   </sortState>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>